<commit_message>
US-9466 [IMP] RR inventory review: months of supply (RR-AMC/FMC) and projected MX (month) displayed with a maximum of 2 digits
</commit_message>
<xml_diff>
--- a/bin/addons/procurement_cycle/report_doc/replenishment_inventory_review.xlsx
+++ b/bin/addons/procurement_cycle/report_doc/replenishment_inventory_review.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.122.1\partage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -929,17 +929,17 @@
     <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1302,7 +1302,7 @@
       <pane xSplit="3" ySplit="15" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1328,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1401,10 +1401,10 @@
       <c r="AP2" s="1"/>
     </row>
     <row r="3" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
@@ -1444,10 +1444,10 @@
       <c r="AP3" s="1"/>
     </row>
     <row r="4" spans="1:45" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="17" t="s">
         <v>70</v>
       </c>
@@ -1489,10 +1489,10 @@
       <c r="AP4" s="1"/>
     </row>
     <row r="5" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="3">
         <v>44331.423958333333</v>
       </c>
@@ -1534,10 +1534,10 @@
       <c r="AP5" s="1"/>
     </row>
     <row r="6" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="4">
         <v>44197</v>
       </c>
@@ -1579,10 +1579,10 @@
       <c r="AP6" s="1"/>
     </row>
     <row r="7" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="4">
         <v>44316</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="G7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="30">
         <v>0</v>
       </c>
       <c r="I7" s="1"/>
@@ -1624,10 +1624,10 @@
       <c r="AP7" s="1"/>
     </row>
     <row r="8" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="2">
         <v>8</v>
       </c>
@@ -1666,10 +1666,10 @@
       <c r="AP8" s="1"/>
     </row>
     <row r="9" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="30"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="4">
         <v>44561</v>
       </c>
@@ -1707,10 +1707,10 @@
       <c r="AP9" s="1"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="2">
         <v>12</v>
       </c>
@@ -1748,10 +1748,10 @@
       <c r="AP10" s="1"/>
     </row>
     <row r="11" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="6" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
US-10748 [FIX] MML: Put lines in case in case there is a level 2 alert on Product list, Product list consistency, RR Inventory Review and MSR reports. Plus some fixes
</commit_message>
<xml_diff>
--- a/bin/addons/procurement_cycle/report_doc/replenishment_inventory_review.xlsx
+++ b/bin/addons/procurement_cycle/report_doc/replenishment_inventory_review.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.122.1\partage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.123.1\partage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>Inventory Review</t>
   </si>
@@ -213,32 +213,29 @@
     <t>No</t>
   </si>
   <si>
-    <t>style grey</t>
-  </si>
-  <si>
-    <t>percent style</t>
-  </si>
-  <si>
-    <t>float style</t>
-  </si>
-  <si>
-    <t>date style</t>
-  </si>
-  <si>
     <t>30/1/1980</t>
   </si>
   <si>
-    <t>red cell style</t>
-  </si>
-  <si>
     <t xml:space="preserve">Every 1 week(s) on monday  </t>
+  </si>
+  <si>
+    <t>float style, red cell style</t>
+  </si>
+  <si>
+    <t>style grey, style red grey</t>
+  </si>
+  <si>
+    <t>percent style, red percent style</t>
+  </si>
+  <si>
+    <t>date style, red date style</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -400,6 +397,12 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -855,7 +858,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -929,6 +932,30 @@
     <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -938,8 +965,14 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1296,13 +1329,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS16"/>
+  <dimension ref="A1:AS17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="15" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="15" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1361,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="37"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1401,19 +1434,19 @@
       <c r="AP2" s="1"/>
     </row>
     <row r="3" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H3" s="19"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="38"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1444,21 +1477,23 @@
       <c r="AP3" s="1"/>
     </row>
     <row r="4" spans="1:45" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H4" s="21">
         <v>0.12</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="39">
+        <v>0.12</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1489,10 +1524,10 @@
       <c r="AP4" s="1"/>
     </row>
     <row r="5" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="3">
         <v>44331.423958333333</v>
       </c>
@@ -1503,7 +1538,9 @@
       <c r="H5" s="20">
         <v>1.123</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="34">
+        <v>0</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1534,21 +1571,23 @@
       <c r="AP5" s="1"/>
     </row>
     <row r="6" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="4">
         <v>44197</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>64</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1579,20 +1618,15 @@
       <c r="AP6" s="1"/>
     </row>
     <row r="7" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="4">
         <v>44316</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="30">
-        <v>0</v>
-      </c>
+      <c r="G7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1624,10 +1658,10 @@
       <c r="AP7" s="1"/>
     </row>
     <row r="8" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="2">
         <v>8</v>
       </c>
@@ -1666,10 +1700,10 @@
       <c r="AP8" s="1"/>
     </row>
     <row r="9" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="4">
         <v>44561</v>
       </c>
@@ -1707,10 +1741,10 @@
       <c r="AP9" s="1"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="2">
         <v>12</v>
       </c>
@@ -1748,10 +1782,10 @@
       <c r="AP10" s="1"/>
     </row>
     <row r="11" spans="1:45" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
@@ -2142,6 +2176,103 @@
       <c r="AR16" s="17"/>
       <c r="AS16" s="17"/>
     </row>
+    <row r="17" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="28">
+        <v>0</v>
+      </c>
+      <c r="K17" s="28">
+        <v>50</v>
+      </c>
+      <c r="L17" s="29"/>
+      <c r="M17" s="28">
+        <v>17</v>
+      </c>
+      <c r="N17" s="28">
+        <v>131</v>
+      </c>
+      <c r="O17" s="28">
+        <v>148</v>
+      </c>
+      <c r="P17" s="28">
+        <v>121.76</v>
+      </c>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="T17" s="27"/>
+      <c r="U17" s="30">
+        <v>18</v>
+      </c>
+      <c r="V17" s="30">
+        <v>30.310889132500002</v>
+      </c>
+      <c r="W17" s="31">
+        <v>1.7320508075700001</v>
+      </c>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="27">
+        <v>1650</v>
+      </c>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="27"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27"/>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH17" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI17" s="27"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="32"/>
+      <c r="AM17" s="33"/>
+      <c r="AN17" s="33"/>
+      <c r="AO17" s="33">
+        <v>44327</v>
+      </c>
+      <c r="AP17" s="33">
+        <v>44344</v>
+      </c>
+      <c r="AQ17" s="33">
+        <v>44475</v>
+      </c>
+      <c r="AR17" s="27"/>
+      <c r="AS17" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A8:B8"/>

</xml_diff>